<commit_message>
Fixes for the design
</commit_message>
<xml_diff>
--- a/m52tu, m54 PnP/Rev 1.1/BOM (not finished).xlsx
+++ b/m52tu, m54 PnP/Rev 1.1/BOM (not finished).xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m52tu, m54 PnP\Rev 1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52tu, m54 PnP\Rev 1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FDD98B-945F-4731-B278-F06A18C1CCB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BC31EB-8C50-4D01-9F51-20EED4D4D7EA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="1770" windowWidth="23655" windowHeight="14430" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="2025" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VR" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="139">
   <si>
     <t>Value</t>
   </si>
@@ -195,24 +195,6 @@
     <t>311-10.0KHRTR-ND</t>
   </si>
   <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>CAN-bus termination resistor</t>
-  </si>
-  <si>
-    <t>RES SMD 120 OHM 1% 1/8W 0603</t>
-  </si>
-  <si>
-    <t>RC0603FR-07120RL</t>
-  </si>
-  <si>
-    <t>603-RC0603FR-07120RL</t>
-  </si>
-  <si>
-    <t>311-120HRCT-ND</t>
-  </si>
-  <si>
     <t>RES SMD 100K OHM 5% 1/8W 1206</t>
   </si>
   <si>
@@ -454,6 +436,21 @@
   </si>
   <si>
     <t xml:space="preserve">	490-17948-1-ND</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CAP CER 10nF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>603-CC603KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>311-1085-1-ND</t>
   </si>
 </sst>
 </file>
@@ -534,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -594,6 +591,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -651,7 +709,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -674,9 +732,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -696,26 +751,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1115,12 +1210,12 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="11" customWidth="1"/>
     <col min="2" max="2" width="37.375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="53.125" customWidth="1"/>
@@ -1130,11 +1225,11 @@
     <col min="14" max="14" width="47.875" customWidth="1"/>
     <col min="15" max="15" width="27.375" customWidth="1"/>
     <col min="16" max="16" width="28" customWidth="1"/>
-    <col min="17" max="17" width="22.375" customWidth="1"/>
+    <col min="17" max="17" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" thickBot="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1176,18 +1271,18 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="29" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A2" s="11"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1201,18 +1296,19 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4" t="str">
-        <f>IF(NOT(H2=""),A2&amp;","&amp;H2,"")</f>
+      <c r="O2" s="20" t="str">
+        <f t="shared" ref="O2:O24" si="0">IF(NOT(H2=""),A2&amp;","&amp;H2,"")</f>
         <v/>
       </c>
-      <c r="P2" t="str">
+      <c r="P2" s="26" t="str">
         <f>A2&amp;"x "&amp;C2</f>
         <v xml:space="preserve">x </v>
       </c>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A3" s="13">
-        <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
+      <c r="A3" s="12">
+        <f t="shared" ref="A3:A12" si="1">LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1244,30 +1340,30 @@
         <v>0</v>
       </c>
       <c r="L3" s="6">
-        <f>J3*A3</f>
+        <f t="shared" ref="L3:L17" si="2">J3*A3</f>
         <v>0.1</v>
       </c>
       <c r="M3" s="6">
-        <f>K3*A3</f>
+        <f t="shared" ref="M3:M17" si="3">K3*A3</f>
         <v>0</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="4" t="str">
-        <f>IF(NOT(H3=""),A3&amp;","&amp;H3,"")</f>
+      <c r="O3" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>1,311-7.5KERTR-ND</v>
       </c>
-      <c r="P3" t="str">
-        <f>"Resistor - " &amp;A3&amp;"x "&amp;C3</f>
+      <c r="P3" s="26" t="str">
+        <f t="shared" ref="P3:P8" si="4">"Resistor - " &amp;A3&amp;"x "&amp;C3</f>
         <v>Resistor - 1x 7.5k</v>
       </c>
-      <c r="Q3" t="str">
-        <f>IF(NOT(I3=""),I3&amp;"|"&amp;A3,"")</f>
+      <c r="Q3" s="26" t="str">
+        <f t="shared" ref="Q3:Q24" si="5">IF(NOT(I3=""),I3&amp;"|"&amp;A3,"")</f>
         <v>603-RC1206JR-077K5L|1</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="13">
-        <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
+      <c r="A4" s="12">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1299,30 +1395,30 @@
         <v>0</v>
       </c>
       <c r="L4" s="6">
-        <f>J4*A4</f>
+        <f t="shared" si="2"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="M4" s="6">
-        <f>K4*A4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N4" s="4"/>
-      <c r="O4" s="4" t="str">
-        <f>IF(NOT(H4=""),A4&amp;","&amp;H4,"")</f>
+      <c r="O4" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>7,YAG1341TR-ND</v>
       </c>
-      <c r="P4" t="str">
-        <f>"Resistor - " &amp;A4&amp;"x "&amp;C4</f>
+      <c r="P4" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>Resistor - 7x 1k</v>
       </c>
-      <c r="Q4" t="str">
-        <f>IF(NOT(I4=""),I4&amp;"|"&amp;A4,"")</f>
+      <c r="Q4" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-RC1206JR-071KP|7</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A5" s="13">
-        <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
+      <c r="A5" s="12">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1354,30 +1450,30 @@
         <v>0</v>
       </c>
       <c r="L5" s="6">
-        <f>J5*A5</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="M5" s="6">
-        <f>K5*A5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="4" t="str">
-        <f>IF(NOT(H5=""),A5&amp;","&amp;H5,"")</f>
+      <c r="O5" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>1,311-2.00KFRTR-ND</v>
       </c>
-      <c r="P5" t="str">
-        <f>"Resistor - " &amp;A5&amp;"x "&amp;C5</f>
+      <c r="P5" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>Resistor - 1x 2k</v>
       </c>
-      <c r="Q5" t="str">
-        <f>IF(NOT(I5=""),I5&amp;"|"&amp;A5,"")</f>
+      <c r="Q5" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-RC1206FR-072KL|1</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A6" s="13">
-        <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
+      <c r="A6" s="12">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1399,7 +1495,7 @@
       <c r="H6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="15" t="s">
         <v>51</v>
       </c>
       <c r="J6" s="5">
@@ -1409,30 +1505,30 @@
         <v>0</v>
       </c>
       <c r="L6" s="6">
-        <f>J6*A6</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="M6" s="6">
-        <f>K6*A6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N6" s="4"/>
-      <c r="O6" s="4" t="str">
-        <f>IF(NOT(H6=""),A6&amp;","&amp;H6,"")</f>
+      <c r="O6" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>2,311-10.0KHRTR-ND</v>
       </c>
-      <c r="P6" t="str">
-        <f>"Resistor - " &amp;A6&amp;"x "&amp;C6</f>
+      <c r="P6" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>Resistor - 2x 10k</v>
       </c>
-      <c r="Q6" t="str">
-        <f>IF(NOT(I6=""),I6&amp;"|"&amp;A6,"")</f>
+      <c r="Q6" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-RC0603FR-0710KL|2</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A7" s="13">
-        <f>LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+      <c r="A7" s="12">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1442,158 +1538,122 @@
         <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J7" s="5">
         <v>0.2</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="6">
-        <f>J7*A7</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="M7" s="6">
-        <f>K7*A7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N7" s="4"/>
-      <c r="O7" s="4" t="str">
-        <f>IF(NOT(H7=""),A7&amp;","&amp;H7,"")</f>
+      <c r="O7" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>4,YAG3912CT-ND</v>
       </c>
-      <c r="P7" t="str">
-        <f>"Resistor - " &amp;A7&amp;"x "&amp;C7</f>
+      <c r="P7" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>Resistor - 4x 100k</v>
       </c>
-      <c r="Q7" t="str">
-        <f>IF(NOT(I7=""),I7&amp;"|"&amp;A7,"")</f>
+      <c r="Q7" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-AC1206JR-07100KL|4</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A8" s="13">
-        <f>LEN(B8)-LEN(SUBSTITUTE(B8,",",""))+1</f>
+      <c r="A8" s="12">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J8" s="5">
         <v>0.2</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6">
-        <f>J8*A8</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="M8" s="6">
-        <f>K8*A8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="4" t="str">
-        <f>IF(NOT(H8=""),A8&amp;","&amp;H8,"")</f>
+      <c r="O8" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>1,311-4.7KGRCT-ND</v>
       </c>
-      <c r="P8" t="str">
-        <f>"Resistor - " &amp;A8&amp;"x "&amp;C8</f>
+      <c r="P8" s="26" t="str">
+        <f t="shared" si="4"/>
         <v>Resistor - 1x 4.7k</v>
       </c>
-      <c r="Q8" t="str">
-        <f>IF(NOT(I8=""),I8&amp;"|"&amp;A8,"")</f>
+      <c r="Q8" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-RC0603JR-074K7L|1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="39" thickBot="1">
-      <c r="A9" s="13">
-        <f>LEN(B9)-LEN(SUBSTITUTE(B9,",",""))+1</f>
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="3">
-        <v>120</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.2</v>
-      </c>
+    <row r="9" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="6">
-        <f>J9*A9</f>
-        <v>0.2</v>
-      </c>
-      <c r="M9" s="6">
-        <f>K9*A9</f>
-        <v>0</v>
-      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4" t="str">
-        <f>IF(NOT(H9=""),A9&amp;","&amp;H9,"")</f>
-        <v>1,311-120HRCT-ND</v>
-      </c>
-      <c r="P9" t="str">
-        <f>"Resistor - " &amp;A9&amp;"x "&amp;C9</f>
-        <v>Resistor - 1x 120</v>
-      </c>
-      <c r="Q9" t="str">
-        <f>IF(NOT(I9=""),I9&amp;"|"&amp;A9,"")</f>
-        <v>603-RC0603FR-07120RL|1</v>
-      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A10" s="13">
-        <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
+      <c r="A10" s="12">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1603,20 +1663,20 @@
         <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J10" s="5">
         <v>0.1</v>
@@ -1625,30 +1685,30 @@
         <v>0</v>
       </c>
       <c r="L10" s="6">
-        <f>J10*A10</f>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="M10" s="6">
-        <f>K10*A10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N10" s="4"/>
-      <c r="O10" s="4" t="str">
-        <f>IF(NOT(H10=""),A10&amp;","&amp;H10,"")</f>
+      <c r="O10" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>5,311-1343-1-ND</v>
       </c>
-      <c r="P10" t="str">
-        <f>"Capacitor - " &amp;A10&amp;"x "&amp;C10</f>
+      <c r="P10" s="26" t="str">
+        <f t="shared" ref="P10:P17" si="6">"Capacitor - " &amp;A10&amp;"x "&amp;C10</f>
         <v>Capacitor - 5x 0.1uF</v>
       </c>
-      <c r="Q10" t="str">
-        <f>IF(NOT(I10=""),I10&amp;"|"&amp;A10,"")</f>
+      <c r="Q10" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-CC603ZPY5V9BB104|5</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A11" s="13">
-        <f>LEN(B11)-LEN(SUBSTITUTE(B11,",",""))+1</f>
+      <c r="A11" s="12">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1658,20 +1718,20 @@
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>67</v>
       </c>
       <c r="J11" s="5">
         <v>0.1</v>
@@ -1680,393 +1740,396 @@
         <v>0</v>
       </c>
       <c r="L11" s="6">
-        <f>J11*A11</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="M11" s="6">
-        <f>K11*A11</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N11" s="4"/>
-      <c r="O11" s="4" t="str">
-        <f>IF(NOT(H11=""),A11&amp;","&amp;H11,"")</f>
+      <c r="O11" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>1,311-1963-1-ND</v>
       </c>
-      <c r="P11" t="str">
-        <f>"Capacitor - " &amp;A11&amp;"x "&amp;C11</f>
+      <c r="P11" s="26" t="str">
+        <f t="shared" si="6"/>
         <v>Capacitor - 1x 1uF</v>
       </c>
-      <c r="Q11" t="str">
-        <f>IF(NOT(I11=""),I11&amp;"|"&amp;A11,"")</f>
+      <c r="Q11" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>603-CC126KKX7R9BB105|1</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="13">
-        <f t="shared" ref="A12" si="0">LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
+      <c r="A12" s="12">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="5">
+        <v>63</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="31">
         <v>0.1</v>
       </c>
       <c r="K12" s="5">
         <v>0</v>
       </c>
       <c r="L12" s="6">
-        <f>J12*A12</f>
+        <f t="shared" ref="L12" si="7">J12*A12</f>
         <v>0.1</v>
       </c>
       <c r="M12" s="6">
-        <f>K12*A12</f>
+        <f t="shared" ref="M12" si="8">K12*A12</f>
         <v>0</v>
       </c>
       <c r="N12" s="4"/>
-      <c r="O12" s="4" t="str">
-        <f>IF(NOT(H12=""),A12&amp;","&amp;H12,"")</f>
+      <c r="O12" s="20" t="str">
+        <f t="shared" ref="O12" si="9">IF(NOT(H12=""),A12&amp;","&amp;H12,"")</f>
         <v>1,311-1174-1-ND</v>
       </c>
-      <c r="P12" t="str">
-        <f>"Capacitor - " &amp;A12&amp;"x "&amp;C12</f>
+      <c r="P12" s="26" t="str">
+        <f t="shared" ref="P12" si="10">"Capacitor - " &amp;A12&amp;"x "&amp;C12</f>
         <v>Capacitor - 1x 10nF</v>
       </c>
-      <c r="Q12" t="str">
-        <f>IF(NOT(I12=""),I12&amp;"|"&amp;A12,"")</f>
+      <c r="Q12" s="26" t="str">
+        <f t="shared" ref="Q12" si="11">IF(NOT(I12=""),I12&amp;"|"&amp;A12,"")</f>
         <v>603-CC206KRX7R9BB103|1</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A13" s="13">
-        <f t="shared" ref="A13" si="1">LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
-        <v>1</v>
+      <c r="A13" s="12">
+        <f t="shared" ref="A13" si="12">LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>134</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="5">
+        <v>136</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="31">
         <v>0.1</v>
       </c>
       <c r="K13" s="5">
         <v>0</v>
       </c>
       <c r="L13" s="6">
-        <f>J13*A13</f>
-        <v>0.1</v>
+        <f t="shared" si="2"/>
+        <v>0.2</v>
       </c>
       <c r="M13" s="6">
-        <f>K13*A13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N13" s="4"/>
-      <c r="O13" s="4" t="str">
-        <f>IF(NOT(H13=""),A13&amp;","&amp;H13,"")</f>
-        <v>1,1830-1079-1-ND</v>
-      </c>
-      <c r="P13" t="str">
-        <f>"Capacitor - " &amp;A13&amp;"x "&amp;C13</f>
-        <v xml:space="preserve">Capacitor - 1x </v>
-      </c>
-      <c r="Q13" t="str">
-        <f>IF(NOT(I13=""),I13&amp;"|"&amp;A13,"")</f>
-        <v>743-IN-S85ATG|1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A14" s="13">
-        <f t="shared" ref="A14:A15" si="2">LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
+      <c r="O13" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>2,311-1085-1-ND</v>
+      </c>
+      <c r="P13" s="26" t="str">
+        <f t="shared" si="6"/>
+        <v>Capacitor - 2x 10nF</v>
+      </c>
+      <c r="Q13" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>603-CC603KRX7R9BB103|2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A14" s="12">
+        <f t="shared" ref="A14" si="13">LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="J14" s="5">
+        <v>114</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="31">
         <v>0.1</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
       </c>
       <c r="L14" s="6">
-        <f>J14*A14</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="M14" s="6">
-        <f>K14*A14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14" s="4"/>
-      <c r="O14" s="4" t="str">
-        <f>IF(NOT(H14=""),A14&amp;","&amp;H14,"")</f>
-        <v/>
-      </c>
-      <c r="P14" t="str">
-        <f>"Capacitor - " &amp;A14&amp;"x "&amp;C14</f>
+      <c r="O14" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>1,1830-1079-1-ND</v>
+      </c>
+      <c r="P14" s="26" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Capacitor - 1x </v>
       </c>
-      <c r="Q14" t="str">
-        <f>IF(NOT(I14=""),I14&amp;"|"&amp;A14,"")</f>
-        <v>583-FM4004W-W|1</v>
+      <c r="Q14" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>743-IN-S85ATG|1</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A15" s="13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+      <c r="A15" s="12">
+        <f t="shared" ref="A15:A16" si="14">LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="J15" s="5">
+        <v>126</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="31">
         <v>0.1</v>
       </c>
       <c r="K15" s="5">
         <v>0</v>
       </c>
       <c r="L15" s="6">
-        <f>J15*A15</f>
-        <v>0.2</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="M15" s="6">
-        <f>K15*A15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N15" s="4"/>
-      <c r="O15" s="4" t="str">
-        <f>IF(NOT(H15=""),A15&amp;","&amp;H15,"")</f>
-        <v>2,	490-17948-1-ND</v>
-      </c>
-      <c r="P15" t="str">
-        <f>"Capacitor - " &amp;A15&amp;"x "&amp;C15</f>
-        <v xml:space="preserve">Capacitor - 2x </v>
-      </c>
-      <c r="Q15" t="str">
-        <f>IF(NOT(I15=""),I15&amp;"|"&amp;A15,"")</f>
-        <v>81-CSTNE16M0V530000R|2</v>
+      <c r="O15" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P15" s="26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">Capacitor - 1x </v>
+      </c>
+      <c r="Q15" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>583-FM4004W-W|1</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A16" s="13">
-        <f t="shared" ref="A16" si="3">LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
-        <v>1</v>
+      <c r="A16" s="12">
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="5">
+        <v>130</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="J16" s="31">
         <v>0.1</v>
       </c>
       <c r="K16" s="5">
         <v>0</v>
       </c>
       <c r="L16" s="6">
-        <f>J16*A16</f>
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>2,	490-17948-1-ND</v>
+      </c>
+      <c r="P16" s="26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">Capacitor - 2x </v>
+      </c>
+      <c r="Q16" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>81-CSTNE16M0V530000R|2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A17" s="12">
+        <f t="shared" ref="A17" si="15">LEN(B17)-LEN(SUBSTITUTE(B17,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="31">
         <v>0.1</v>
       </c>
-      <c r="M16" s="6">
-        <f>K16*A16</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4" t="str">
-        <f>IF(NOT(H16=""),A16&amp;","&amp;H16,"")</f>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="O17" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>1,507-2450-1-ND</v>
       </c>
-      <c r="P16" t="str">
-        <f>"Capacitor - " &amp;A16&amp;"x "&amp;C16</f>
+      <c r="P17" s="26" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">Capacitor - 1x </v>
       </c>
-      <c r="Q16" t="str">
-        <f>IF(NOT(I16=""),I16&amp;"|"&amp;A16,"")</f>
+      <c r="Q17" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>530-0685P5000-01|1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4" t="str">
-        <f>IF(NOT(H17=""),A17&amp;","&amp;H17,"")</f>
+    <row r="18" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="20" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q17" t="str">
-        <f>IF(NOT(I17=""),I17&amp;"|"&amp;A17,"")</f>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A18" s="13">
-        <f>LEN(B18)-LEN(SUBSTITUTE(B18,",",""))+1</f>
+    <row r="19" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A19" s="12">
+        <f t="shared" ref="A19:A24" si="16">LEN(B19)-LEN(SUBSTITUTE(B19,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J18" s="5">
-        <v>1.94</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0</v>
-      </c>
-      <c r="L18" s="6">
-        <f>J18*A18</f>
-        <v>1.94</v>
-      </c>
-      <c r="M18" s="6">
-        <f>K18*A18</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4" t="str">
-        <f>IF(NOT(H18=""),A18&amp;","&amp;H18,"")</f>
-        <v>1,NSVMMBT2222ATT1GOSCT-ND</v>
-      </c>
-      <c r="P18" t="str">
-        <f>"IC- " &amp;A18&amp;"x "&amp;C18</f>
-        <v xml:space="preserve">IC- 1x </v>
-      </c>
-      <c r="Q18" t="str">
-        <f>IF(NOT(I18=""),I18&amp;"|"&amp;A18,"")</f>
-        <v>863-MMBT2222ATT1G|1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A19" s="13">
-        <f>LEN(B19)-LEN(SUBSTITUTE(B19,",",""))+1</f>
-        <v>6</v>
-      </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="22"/>
       <c r="F19" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="J19" s="5">
         <v>1.94</v>
@@ -2075,106 +2138,104 @@
         <v>0</v>
       </c>
       <c r="L19" s="6">
-        <f>J19*A19</f>
+        <f t="shared" ref="L19:L24" si="17">J19*A19</f>
+        <v>1.94</v>
+      </c>
+      <c r="M19" s="6">
+        <f t="shared" ref="M19:M24" si="18">K19*A19</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>1,NSVMMBT2222ATT1GOSCT-ND</v>
+      </c>
+      <c r="P19" s="26" t="str">
+        <f>"IC- " &amp;A19&amp;"x "&amp;C19</f>
+        <v xml:space="preserve">IC- 1x </v>
+      </c>
+      <c r="Q19" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>863-MMBT2222ATT1G|1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A20" s="12">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1.94</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="17"/>
         <v>11.64</v>
       </c>
-      <c r="M19" s="6">
-        <f>K19*A19</f>
-        <v>0</v>
-      </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4" t="str">
-        <f>IF(NOT(H19=""),A19&amp;","&amp;H19,"")</f>
+      <c r="M20" s="6">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="20" t="str">
+        <f t="shared" si="0"/>
         <v>6,ISL9V3040S3STCT-ND</v>
       </c>
-      <c r="P19" t="str">
-        <f>"IC- " &amp;A19&amp;"x "&amp;C19</f>
+      <c r="P20" s="26" t="str">
+        <f>"IC- " &amp;A20&amp;"x "&amp;C20</f>
         <v xml:space="preserve">IC- 6x </v>
       </c>
-      <c r="Q19" t="str">
-        <f>IF(NOT(I19=""),I19&amp;"|"&amp;A19,"")</f>
+      <c r="Q20" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>512-ISL9V3040S3ST|6</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A20" s="13">
-        <f>LEN(B20)-LEN(SUBSTITUTE(B20,",",""))+1</f>
+    <row r="21" spans="1:17" ht="16.5" thickBot="1">
+      <c r="A21" s="12">
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K20" s="5">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
-        <f>J20*A20</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="M20" s="6">
-        <f>K20*A20</f>
-        <v>0</v>
-      </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4" t="str">
-        <f>IF(NOT(H20=""),A20&amp;","&amp;H20,"")</f>
-        <v>2,497-14323-1-ND</v>
-      </c>
-      <c r="P20" t="str">
-        <f>"Pins- " &amp;A20&amp;"x "&amp;C20</f>
-        <v xml:space="preserve">Pins- 2x </v>
-      </c>
-      <c r="Q20" t="str">
-        <f>IF(NOT(I20=""),I20&amp;"|"&amp;A20,"")</f>
-        <v>511-VNLD5090TR-E|2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A21" s="13">
-        <f>LEN(B21)-LEN(SUBSTITUTE(B21,",",""))+1</f>
-        <v>1</v>
-      </c>
       <c r="B21" s="4" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>90</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>92</v>
+        <v>107</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>108</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="J21" s="5">
         <v>0.14000000000000001</v>
@@ -2183,53 +2244,53 @@
         <v>0</v>
       </c>
       <c r="L21" s="6">
-        <f>J21*A21</f>
-        <v>0.14000000000000001</v>
+        <f t="shared" si="17"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M21" s="6">
-        <f>K21*A21</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N21" s="4"/>
-      <c r="O21" s="4" t="str">
-        <f>IF(NOT(H21=""),A21&amp;","&amp;H21,"")</f>
-        <v>1,ATMEGA328P-AURCT-ND</v>
-      </c>
-      <c r="P21" t="str">
+      <c r="O21" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>2,497-14323-1-ND</v>
+      </c>
+      <c r="P21" s="26" t="str">
         <f>"Pins- " &amp;A21&amp;"x "&amp;C21</f>
-        <v xml:space="preserve">Pins- 1x </v>
-      </c>
-      <c r="Q21" t="str">
-        <f>IF(NOT(I21=""),I21&amp;"|"&amp;A21,"")</f>
-        <v>556-ATMEGA328P-AU|1</v>
+        <v xml:space="preserve">Pins- 2x </v>
+      </c>
+      <c r="Q21" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>511-VNLD5090TR-E|2</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A22" s="13">
-        <f>LEN(B22)-LEN(SUBSTITUTE(B22,",",""))+1</f>
+      <c r="A22" s="12">
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="I22" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="J22" s="5">
         <v>0.14000000000000001</v>
@@ -2238,53 +2299,53 @@
         <v>0</v>
       </c>
       <c r="L22" s="6">
-        <f>J22*A22</f>
+        <f t="shared" si="17"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="M22" s="6">
-        <f>K22*A22</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="4" t="str">
-        <f>IF(NOT(H22=""),A22&amp;","&amp;H22,"")</f>
-        <v>1,MCP2515-I/SO-ND</v>
-      </c>
-      <c r="P22" t="str">
+      <c r="O22" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>1,ATMEGA328P-AURCT-ND</v>
+      </c>
+      <c r="P22" s="26" t="str">
         <f>"Pins- " &amp;A22&amp;"x "&amp;C22</f>
         <v xml:space="preserve">Pins- 1x </v>
       </c>
-      <c r="Q22" t="str">
-        <f>IF(NOT(I22=""),I22&amp;"|"&amp;A22,"")</f>
-        <v>579-MCP2515-I/SO|1</v>
+      <c r="Q22" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>556-ATMEGA328P-AU|1</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A23" s="13">
-        <f>LEN(B23)-LEN(SUBSTITUTE(B23,",",""))+1</f>
+      <c r="A23" s="12">
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="J23" s="5">
         <v>0.14000000000000001</v>
@@ -2293,49 +2354,53 @@
         <v>0</v>
       </c>
       <c r="L23" s="6">
-        <f>J23*A23</f>
+        <f t="shared" si="17"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="M23" s="6">
-        <f>K23*A23</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N23" s="4"/>
-      <c r="O23" s="4" t="str">
-        <f>IF(NOT(H23=""),A23&amp;","&amp;H23,"")</f>
-        <v>1,MCP2551T-I/SNCT-ND</v>
-      </c>
-      <c r="P23" t="str">
+      <c r="O23" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>1,MCP2515-I/SO-ND</v>
+      </c>
+      <c r="P23" s="26" t="str">
         <f>"Pins- " &amp;A23&amp;"x "&amp;C23</f>
         <v xml:space="preserve">Pins- 1x </v>
       </c>
-      <c r="Q23" t="str">
-        <f>IF(NOT(I23=""),I23&amp;"|"&amp;A23,"")</f>
-        <v>579-MCP2551T-I/SN|1</v>
+      <c r="Q23" s="26" t="str">
+        <f t="shared" si="5"/>
+        <v>579-MCP2515-I/SO|1</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A24" s="13">
-        <f>LEN(B24)-LEN(SUBSTITUTE(B24,",",""))+1</f>
+      <c r="A24" s="12">
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="E24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="J24" s="5">
         <v>0.14000000000000001</v>
@@ -2344,73 +2409,76 @@
         <v>0</v>
       </c>
       <c r="L24" s="6">
-        <f>J24*A24</f>
+        <f t="shared" si="17"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="M24" s="6">
-        <f>K24*A24</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N24" s="4"/>
-      <c r="O24" s="4" t="str">
-        <f>IF(NOT(H24=""),A24&amp;","&amp;H24,"")</f>
+      <c r="O24" s="27" t="str">
+        <f t="shared" si="0"/>
         <v>1,MCP2551T-I/SNCT-ND</v>
       </c>
-      <c r="P24" t="str">
+      <c r="P24" s="26" t="str">
         <f>"Pins- " &amp;A24&amp;"x "&amp;C24</f>
         <v xml:space="preserve">Pins- 1x </v>
       </c>
-      <c r="Q24" t="str">
-        <f>IF(NOT(I24=""),I24&amp;"|"&amp;A24,"")</f>
+      <c r="Q24" s="26" t="str">
+        <f t="shared" si="5"/>
         <v>579-MCP2551T-I/SN|1</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A25" s="13">
-        <v>6</v>
-      </c>
+      <c r="A25" s="12"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="22"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
     </row>
     <row r="26" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A26" s="11"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="15"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="14"/>
       <c r="J26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="9">
-        <f>SUM(L2:L23)</f>
+      <c r="L26" s="8">
+        <f>SUM(L2:L24)</f>
         <v>17.780000000000005</v>
       </c>
-      <c r="M26" s="9">
-        <f>SUM(M2:M23)</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="8" t="s">
+      <c r="M26" s="8">
+        <f>SUM(M2:M24)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="21" t="s">
         <v>12</v>
       </c>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>